<commit_message>
Having a little trouble with the process js file
</commit_message>
<xml_diff>
--- a/cos/cos-spotlight.xlsx
+++ b/cos/cos-spotlight.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garza/Development-vpaa/csv-tool/cos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmk424/Documents/GitHub/csv-tool/cos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0B43E8-9536-E542-942E-F18718020FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB92531-DC19-0A44-A56F-9C46E823FDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="500" windowWidth="42520" windowHeight="27780" activeTab="4" xr2:uid="{6667F635-3644-E445-B6D0-C5A8645CA96F}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="20080" activeTab="1" xr2:uid="{6667F635-3644-E445-B6D0-C5A8645CA96F}"/>
   </bookViews>
   <sheets>
     <sheet name="spotlights" sheetId="1" r:id="rId1"/>
     <sheet name="staff" sheetId="4" r:id="rId2"/>
-    <sheet name="student" sheetId="5" r:id="rId3"/>
-    <sheet name="faculty" sheetId="3" r:id="rId4"/>
-    <sheet name="alumni" sheetId="2" r:id="rId5"/>
+    <sheet name="news" sheetId="6" r:id="rId3"/>
+    <sheet name="student" sheetId="5" r:id="rId4"/>
+    <sheet name="faculty" sheetId="3" r:id="rId5"/>
+    <sheet name="alumni" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="561">
   <si>
     <t>Year</t>
   </si>
@@ -4028,7 +4029,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4146,11 +4147,104 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4170,7 +4264,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4182,19 +4279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4206,47 +4291,44 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4256,455 +4338,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="63">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -4943,6 +4576,455 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5137,69 +5219,69 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5A39AD2-E942-AC4C-8DD2-0E833E40C844}" name="Table845" displayName="Table845" ref="A1:N17" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E5A39AD2-E942-AC4C-8DD2-0E833E40C844}" name="Table845" displayName="Table845" ref="A1:N17" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:N17" xr:uid="{E5A39AD2-E942-AC4C-8DD2-0E833E40C844}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{27C4EF48-631B-FB4A-A55B-1E5ABA5D42D8}" name="COS Spotlight Pages (homepage links to Alumni, Faculty, Staff, and Student spotlights; News Spotlights are for news item links)" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{37D36734-188E-994F-839D-97B28E51033E}" name="Year" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{50CE02B7-5205-5645-9950-6D36F8BDF91B}" name="Month" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{FCCFA97E-C91E-1E49-B701-D3E3F94713DC}" name="Source URL" dataDxfId="26" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{693A8A51-DBCC-644F-9332-094E8FEEB0DB}" name="uri" dataDxfId="25" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{03E31006-10A7-F44D-B05F-E38E700A11E4}" name="Cascade URL" dataDxfId="24" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{D3359B64-3848-8B4F-A739-77EC88812713}" name="page type" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{59345FA9-72DA-6946-88D8-4F2D10688EA6}" name="classification" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{EE85ED35-E5E0-3241-B053-F48015BA419F}" name="tags" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{D646E26E-787A-964B-B3B8-80E9FCACA69E}" name="department/discipline" dataDxfId="20" dataCellStyle="Bad"/>
-    <tableColumn id="13" xr3:uid="{361DB3FF-0032-B046-A020-9B1DD554A0AC}" name="image" dataDxfId="19" dataCellStyle="Bad"/>
-    <tableColumn id="10" xr3:uid="{08B1BB45-1062-0A47-A99F-811C82562DD9}" name="notes" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{7E76A756-A4F8-9042-B7D3-D1E7FE5925A1}" name="Notes2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{34DB9956-EF17-0D40-9BE2-3505849C4555}" name="parentFolderPath" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{27C4EF48-631B-FB4A-A55B-1E5ABA5D42D8}" name="COS Spotlight Pages (homepage links to Alumni, Faculty, Staff, and Student spotlights; News Spotlights are for news item links)" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{37D36734-188E-994F-839D-97B28E51033E}" name="Year" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{50CE02B7-5205-5645-9950-6D36F8BDF91B}" name="Month" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{FCCFA97E-C91E-1E49-B701-D3E3F94713DC}" name="Source URL" dataDxfId="41" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{693A8A51-DBCC-644F-9332-094E8FEEB0DB}" name="uri" dataDxfId="40" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{03E31006-10A7-F44D-B05F-E38E700A11E4}" name="Cascade URL" dataDxfId="39" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{D3359B64-3848-8B4F-A739-77EC88812713}" name="page type" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{59345FA9-72DA-6946-88D8-4F2D10688EA6}" name="classification" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{EE85ED35-E5E0-3241-B053-F48015BA419F}" name="tags" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{D646E26E-787A-964B-B3B8-80E9FCACA69E}" name="department/discipline" dataDxfId="35" dataCellStyle="Bad"/>
+    <tableColumn id="13" xr3:uid="{361DB3FF-0032-B046-A020-9B1DD554A0AC}" name="image" dataDxfId="34" dataCellStyle="Bad"/>
+    <tableColumn id="10" xr3:uid="{08B1BB45-1062-0A47-A99F-811C82562DD9}" name="notes" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{7E76A756-A4F8-9042-B7D3-D1E7FE5925A1}" name="Notes2" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{34DB9956-EF17-0D40-9BE2-3505849C4555}" name="parentFolderPath" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0BB935DC-0DCB-C34E-82A6-C2388AC72619}" name="Table8456" displayName="Table8456" ref="A1:N52" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0BB935DC-0DCB-C34E-82A6-C2388AC72619}" name="Table8456" displayName="Table8456" ref="A1:N52" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:N52" xr:uid="{0BB935DC-0DCB-C34E-82A6-C2388AC72619}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{6BFB9FA0-95E7-EA49-B92D-1FF83A61D778}" name="COS Spotlight Pages (homepage links to Alumni, Faculty, Staff, and Student spotlights; News Spotlights are for news item links)" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{9B33FB59-ECD0-BB4D-9F82-15F0E05AB207}" name="Year" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{80C8B957-2225-1048-8314-D84B63B71232}" name="Month" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{970156F2-52D5-6A49-91DA-BF2EFDA2D862}" name="Source URL" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{61CA3668-1E2A-2E4F-A45F-ECB6D357BF3F}" name="uri" dataDxfId="9" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{5DFB6428-5BF6-E449-AB61-C74CFE14F3CD}" name="Cascade URL" dataDxfId="8" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{D018728D-7195-D143-9499-23F48754344C}" name="page type" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{67D7DEAC-B48E-7D43-BAD7-489BFBCC738B}" name="classification" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{0675320E-F914-D041-AF35-E098629490C3}" name="tags" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{DCD850D9-E98F-A64C-A83A-84A2EA1BEFAA}" name="department/discipline" dataDxfId="4" dataCellStyle="Bad"/>
-    <tableColumn id="13" xr3:uid="{850C6E3A-6700-344F-A5B1-A710F38DC482}" name="image" dataDxfId="3" dataCellStyle="Bad"/>
-    <tableColumn id="10" xr3:uid="{E70CE714-4C73-624D-AA5C-EA7BDFB0C2E3}" name="notes" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{DA79CAFD-D29F-F046-8BD1-AEA6563002DF}" name="Notes2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{717A45E7-A37B-E444-81EA-996B5F0DB81D}" name="parentFolderPath" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6BFB9FA0-95E7-EA49-B92D-1FF83A61D778}" name="COS Spotlight Pages (homepage links to Alumni, Faculty, Staff, and Student spotlights; News Spotlights are for news item links)" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{9B33FB59-ECD0-BB4D-9F82-15F0E05AB207}" name="Year" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{80C8B957-2225-1048-8314-D84B63B71232}" name="Month" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{970156F2-52D5-6A49-91DA-BF2EFDA2D862}" name="Source URL" dataDxfId="25" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{61CA3668-1E2A-2E4F-A45F-ECB6D357BF3F}" name="uri" dataDxfId="24" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{5DFB6428-5BF6-E449-AB61-C74CFE14F3CD}" name="Cascade URL" dataDxfId="23" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{D018728D-7195-D143-9499-23F48754344C}" name="page type" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{67D7DEAC-B48E-7D43-BAD7-489BFBCC738B}" name="classification" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{0675320E-F914-D041-AF35-E098629490C3}" name="tags" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{DCD850D9-E98F-A64C-A83A-84A2EA1BEFAA}" name="department/discipline" dataDxfId="19" dataCellStyle="Bad"/>
+    <tableColumn id="13" xr3:uid="{850C6E3A-6700-344F-A5B1-A710F38DC482}" name="image" dataDxfId="18" dataCellStyle="Bad"/>
+    <tableColumn id="10" xr3:uid="{E70CE714-4C73-624D-AA5C-EA7BDFB0C2E3}" name="notes" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{DA79CAFD-D29F-F046-8BD1-AEA6563002DF}" name="Notes2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{717A45E7-A37B-E444-81EA-996B5F0DB81D}" name="parentFolderPath" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0052B200-BCE2-DD4B-98CD-1417E0B05060}" name="Table2" displayName="Table2" ref="A1:N19" totalsRowShown="0" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0052B200-BCE2-DD4B-98CD-1417E0B05060}" name="Table2" displayName="Table2" ref="A1:N19" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:N19" xr:uid="{0052B200-BCE2-DD4B-98CD-1417E0B05060}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{944FA098-D732-EB4E-B5CB-05C0A091A146}" name="COS Spotlight Pages (homepage links to Alumni, Faculty, Staff, and Student spotlights; News Spotlights are for news item links)" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{9E4B1C07-91F5-F64C-8EB3-B13FB6116FE8}" name="Year" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{5A72C1F6-253E-E54D-917E-CB34059784BF}" name="Month" dataDxfId="44" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{480C0533-CD6B-B646-B684-87B90798C426}" name="Source URL" dataDxfId="43" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" xr3:uid="{F3E79359-7FF2-3344-8C65-C2508748C5FC}" name="uri" dataDxfId="42" dataCellStyle="Hyperlink"/>
-    <tableColumn id="6" xr3:uid="{F181E6E1-AA20-0D49-9368-ADDA9E0ABB65}" name="Cascade URL" dataDxfId="41" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{E31326A9-AFD3-F244-8463-5588E9ABC00B}" name="page type" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{49B567AC-FF2B-8148-8750-DC0DDCBF1756}" name="classification" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{BFDC4C08-A940-FE4B-A46D-884626F72311}" name="tags" dataDxfId="38" dataCellStyle="Bad"/>
-    <tableColumn id="10" xr3:uid="{4076D476-24A3-F445-9449-7A35F5031B6D}" name="department/discipline" dataDxfId="37" dataCellStyle="Bad"/>
-    <tableColumn id="11" xr3:uid="{36632D5A-569F-9048-911C-C9B5D4CAA92A}" name="image" dataDxfId="36" dataCellStyle="Bad"/>
-    <tableColumn id="12" xr3:uid="{9B62F545-E339-C649-8530-36555456CDF4}" name="notes" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{E1C215F8-02D2-9347-9B60-5E01FC3550D6}" name="Notes2" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{F063CABE-A16D-B841-AD67-1863BABE02D8}" name="parentFolderPath" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{944FA098-D732-EB4E-B5CB-05C0A091A146}" name="COS Spotlight Pages (homepage links to Alumni, Faculty, Staff, and Student spotlights; News Spotlights are for news item links)" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{9E4B1C07-91F5-F64C-8EB3-B13FB6116FE8}" name="Year" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{5A72C1F6-253E-E54D-917E-CB34059784BF}" name="Month" dataDxfId="11" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{480C0533-CD6B-B646-B684-87B90798C426}" name="Source URL" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{F3E79359-7FF2-3344-8C65-C2508748C5FC}" name="uri" dataDxfId="9" dataCellStyle="Hyperlink"/>
+    <tableColumn id="6" xr3:uid="{F181E6E1-AA20-0D49-9368-ADDA9E0ABB65}" name="Cascade URL" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{E31326A9-AFD3-F244-8463-5588E9ABC00B}" name="page type" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{49B567AC-FF2B-8148-8750-DC0DDCBF1756}" name="classification" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{BFDC4C08-A940-FE4B-A46D-884626F72311}" name="tags" dataDxfId="5" dataCellStyle="Bad"/>
+    <tableColumn id="10" xr3:uid="{4076D476-24A3-F445-9449-7A35F5031B6D}" name="department/discipline" dataDxfId="4" dataCellStyle="Bad"/>
+    <tableColumn id="11" xr3:uid="{36632D5A-569F-9048-911C-C9B5D4CAA92A}" name="image" dataDxfId="3" dataCellStyle="Bad"/>
+    <tableColumn id="12" xr3:uid="{9B62F545-E339-C649-8530-36555456CDF4}" name="notes" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{E1C215F8-02D2-9347-9B60-5E01FC3550D6}" name="Notes2" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{F063CABE-A16D-B841-AD67-1863BABE02D8}" name="parentFolderPath" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5504,8 +5586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68348C16-4DDA-3B4C-933D-C2C187C3F794}">
   <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N47" sqref="A1:N47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10146,6 +10228,7 @@
     <hyperlink ref="F81" r:id="rId264" xr:uid="{905117FD-EE92-1C44-BCB5-4FDE378F62D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId265"/>
   </tableParts>
@@ -10156,7 +10239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D08B964-72DD-7A41-83AD-6C1E3A440240}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:N16"/>
     </sheetView>
   </sheetViews>
@@ -10165,6 +10248,7 @@
     <col min="1" max="1" width="64.5" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
     <col min="6" max="6" width="59.6640625" customWidth="1"/>
+    <col min="11" max="11" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -10671,14 +10755,14 @@
       <c r="A16" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="74" t="s">
+      <c r="C16" s="72"/>
+      <c r="D16" s="73" t="s">
         <v>506</v>
       </c>
-      <c r="E16" s="74"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="7" t="s">
         <v>507</v>
       </c>
@@ -10777,11 +10861,668 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7531071-4613-B64B-BF71-742C587A96DC}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="255" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="101" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="101" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="42" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="49"/>
+    </row>
+    <row r="3" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="82"/>
+      <c r="F3" s="83" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="84"/>
+      <c r="I3" s="53" t="s">
+        <v>473</v>
+      </c>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="53"/>
+      <c r="N3" s="55"/>
+    </row>
+    <row r="4" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="86" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4" s="61"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89" t="s">
+        <v>474</v>
+      </c>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="49"/>
+    </row>
+    <row r="5" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="A5" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="64"/>
+      <c r="D5" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="82"/>
+      <c r="F5" s="83" t="s">
+        <v>167</v>
+      </c>
+      <c r="G5" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I5" s="53"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89" t="s">
+        <v>475</v>
+      </c>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="55"/>
+    </row>
+    <row r="6" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="A6" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="66"/>
+      <c r="D6" s="86" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="86"/>
+      <c r="F6" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" s="61"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89" t="s">
+        <v>476</v>
+      </c>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="49"/>
+    </row>
+    <row r="7" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="A7" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="64"/>
+      <c r="D7" s="82" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" s="53"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89" t="s">
+        <v>477</v>
+      </c>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="55"/>
+    </row>
+    <row r="8" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="A8" s="90" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="91"/>
+      <c r="D8" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="86"/>
+      <c r="F8" s="87" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I8" s="61"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89" t="s">
+        <v>478</v>
+      </c>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="49"/>
+    </row>
+    <row r="9" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+      <c r="A9" s="92" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="93" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="93"/>
+      <c r="D9" s="82" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I9" s="53"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89" t="s">
+        <v>479</v>
+      </c>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="55"/>
+    </row>
+    <row r="10" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+      <c r="A10" s="90" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="91"/>
+      <c r="D10" s="86" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="86"/>
+      <c r="F10" s="87" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I10" s="61"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89" t="s">
+        <v>480</v>
+      </c>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="49"/>
+    </row>
+    <row r="11" spans="1:14" ht="144" x14ac:dyDescent="0.2">
+      <c r="A11" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="95"/>
+      <c r="D11" s="96" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="96"/>
+      <c r="F11" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="53"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89" t="s">
+        <v>481</v>
+      </c>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="55"/>
+    </row>
+    <row r="12" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+      <c r="A12" s="90" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="97"/>
+      <c r="D12" s="98" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="98"/>
+      <c r="F12" s="87" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="61"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89" t="s">
+        <v>482</v>
+      </c>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="49"/>
+    </row>
+    <row r="13" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+      <c r="A13" s="92" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="95"/>
+      <c r="D13" s="96" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="96"/>
+      <c r="F13" s="83" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" s="53"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89" t="s">
+        <v>483</v>
+      </c>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="55"/>
+    </row>
+    <row r="14" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A14" s="90" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="97"/>
+      <c r="D14" s="98" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" s="98"/>
+      <c r="F14" s="87" t="s">
+        <v>194</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" s="61"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89" t="s">
+        <v>484</v>
+      </c>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="49"/>
+    </row>
+    <row r="15" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+      <c r="A15" s="92" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="95"/>
+      <c r="D15" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="96"/>
+      <c r="F15" s="83" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I15" s="53"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89" t="s">
+        <v>483</v>
+      </c>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="55"/>
+    </row>
+    <row r="16" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" s="90" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="97"/>
+      <c r="D16" s="98" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="98"/>
+      <c r="F16" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I16" s="61"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89" t="s">
+        <v>485</v>
+      </c>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="49"/>
+    </row>
+    <row r="17" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+      <c r="A17" s="80" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="81"/>
+      <c r="D17" s="82" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="82"/>
+      <c r="F17" s="83" t="s">
+        <v>203</v>
+      </c>
+      <c r="G17" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89" t="s">
+        <v>486</v>
+      </c>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="55"/>
+    </row>
+    <row r="18" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+      <c r="A18" s="99" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="100"/>
+      <c r="D18" s="86" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" s="86"/>
+      <c r="F18" s="87" t="s">
+        <v>206</v>
+      </c>
+      <c r="G18" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" s="61"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89" t="s">
+        <v>487</v>
+      </c>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="49"/>
+    </row>
+    <row r="19" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+      <c r="A19" s="80" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="81"/>
+      <c r="D19" s="82" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="82"/>
+      <c r="F19" s="83" t="s">
+        <v>209</v>
+      </c>
+      <c r="G19" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" s="53"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89" t="s">
+        <v>488</v>
+      </c>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="55"/>
+    </row>
+    <row r="20" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="A20" s="99" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="100"/>
+      <c r="D20" s="86" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" s="86"/>
+      <c r="F20" s="87" t="s">
+        <v>212</v>
+      </c>
+      <c r="G20" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="I20" s="61"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89" t="s">
+        <v>489</v>
+      </c>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="49"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{34170EAF-DA4D-154C-B71A-6F79433981EB}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{C4654B24-946D-5E44-AEB3-610AA55E4176}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{26FC6C8D-1957-4441-BB26-E8F1C9BF9A5D}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{06DC14A1-2DF2-2748-990C-BD4FDCEF1B99}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{A421DA3D-1953-F24B-ABC3-E60831611B50}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{3584A91A-C807-CB42-8B49-FD3FCC10B42A}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{2F18CC00-85B6-F541-934B-CD5238ABCE99}"/>
+    <hyperlink ref="F4:F6" r:id="rId8" display="https://sciences.utsa.edu/spotlight-news/2020/" xr:uid="{A4A01348-6BE2-D54F-B6A7-FC218DF60BEB}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{F9D3EB70-6809-F548-AC1D-3A517863DD8D}"/>
+    <hyperlink ref="F4" r:id="rId10" xr:uid="{D6299FA4-418F-AF4C-AE0A-7BEF82E81F08}"/>
+    <hyperlink ref="F5" r:id="rId11" xr:uid="{144C1CBA-FCEA-1241-BE37-2923B1CEA9E9}"/>
+    <hyperlink ref="D10" r:id="rId12" xr:uid="{B68F6F6F-04B9-994D-A1FF-190C4E1AD99A}"/>
+    <hyperlink ref="D9" r:id="rId13" xr:uid="{D427AF06-4B30-E948-B844-CF1475E5BE41}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{0A5F9A15-C913-8C4C-BF69-B4F86B7317F4}"/>
+    <hyperlink ref="F10" r:id="rId15" xr:uid="{3440FD18-E5A6-7646-B58A-B1208415C36C}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{6929BD5A-161F-314B-AB1E-5CC5F4A23D72}"/>
+    <hyperlink ref="F8" r:id="rId17" xr:uid="{BE13C7C7-F387-324F-8D79-821DB316D4D4}"/>
+    <hyperlink ref="D16" r:id="rId18" xr:uid="{9D659310-41A2-854D-AEB5-D0AD0CC18ECB}"/>
+    <hyperlink ref="D14" r:id="rId19" xr:uid="{55CE3E1D-0922-CD40-9D46-D48ABB40F903}"/>
+    <hyperlink ref="D13" r:id="rId20" xr:uid="{17D7AE7A-D0DE-2043-B34C-15B17FFDBAF6}"/>
+    <hyperlink ref="D15" r:id="rId21" xr:uid="{5FA251F5-2629-D142-80B5-2FC6FF4FA40A}"/>
+    <hyperlink ref="D12" r:id="rId22" xr:uid="{07F3C37D-9005-624C-BD78-A73DDDB6EEF3}"/>
+    <hyperlink ref="D11" r:id="rId23" xr:uid="{52C66C8C-E214-9049-A1EB-A524C9FFF522}"/>
+    <hyperlink ref="F16" r:id="rId24" xr:uid="{BCF06F97-48BF-D447-BCA1-F10934874583}"/>
+    <hyperlink ref="F14:F16" r:id="rId25" display="https://sciences.utsa.edu/spotlight-news/2022/" xr:uid="{C13E41D6-F652-624E-A376-86ABC8B0DF4D}"/>
+    <hyperlink ref="F14" r:id="rId26" xr:uid="{4C42E895-D2BC-334C-88A5-3F2AD853D6DC}"/>
+    <hyperlink ref="F13" r:id="rId27" xr:uid="{A0D1FB31-F1E3-E74E-A9E4-CBF438F4979C}"/>
+    <hyperlink ref="F15" r:id="rId28" xr:uid="{F12F01DE-51D0-8E4B-A524-1AFEC5177006}"/>
+    <hyperlink ref="F12" r:id="rId29" xr:uid="{0707813F-878A-B74E-88DF-EEB30F85B60D}"/>
+    <hyperlink ref="F11" r:id="rId30" xr:uid="{76E68C5B-5730-FB4E-93BB-6EAFC4240A61}"/>
+    <hyperlink ref="D17" r:id="rId31" xr:uid="{DDA47215-B786-3F4F-A355-75FCC985070C}"/>
+    <hyperlink ref="F17" r:id="rId32" xr:uid="{4801938C-48E7-1946-9F26-1D614F269A0D}"/>
+    <hyperlink ref="D18" r:id="rId33" xr:uid="{F1838FBC-E880-DE4D-BA80-87B93D7C7759}"/>
+    <hyperlink ref="F18" r:id="rId34" xr:uid="{F5A72200-FC4E-FF4C-AF18-75691E41EB16}"/>
+    <hyperlink ref="D19" r:id="rId35" xr:uid="{E90E4D36-C38F-8B43-B4DA-1FB4EF677DB1}"/>
+    <hyperlink ref="F19" r:id="rId36" xr:uid="{A4B9916E-E901-CF40-8FD0-2EE19C0E737C}"/>
+    <hyperlink ref="D20" r:id="rId37" xr:uid="{AC8B1EDB-FA4F-6C42-B068-1986996E3BD0}"/>
+    <hyperlink ref="F20" r:id="rId38" xr:uid="{96D1846A-1669-EA49-8941-C14A2D98AC13}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EA4A51-12E0-F540-9B0B-6BB65C5615F3}">
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12659,7 +13400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B721DFFC-8100-7D4A-BFE0-9EA21660A356}">
   <dimension ref="A1:N29"/>
   <sheetViews>
@@ -13218,27 +13959,27 @@
         <v>119</v>
       </c>
       <c r="E17" s="70"/>
-      <c r="F17" s="71" t="s">
+      <c r="F17" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="71" t="s">
+      <c r="G17" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="71" t="s">
+      <c r="I17" s="62" t="s">
         <v>458</v>
       </c>
-      <c r="J17" s="71" t="s">
+      <c r="J17" s="62" t="s">
         <v>459</v>
       </c>
-      <c r="K17" s="71" t="s">
+      <c r="K17" s="62" t="s">
         <v>460</v>
       </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="72"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="71"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="65" t="s">
@@ -13711,11 +14452,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786DD0DC-FCC5-FE4A-A7A7-903913C35855}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>